<commit_message>
Align code with the latest update of Carousell
</commit_message>
<xml_diff>
--- a/CarousellData.xlsx
+++ b/CarousellData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
   <si>
     <t>Unit Name</t>
   </si>
@@ -60,6 +60,166 @@
   </si>
   <si>
     <t>Special Character?</t>
+  </si>
+  <si>
+    <t>Smdc shore 1 Condosharing condoshare bedspace</t>
+  </si>
+  <si>
+    <t>smdc shore 1 
+tower d
+rm734-7th floor
+in front of SM Moa
+need 4person
+p20000/month
+or p5,000 bedspace/per head
+inclusive condo dues
+water &amp; electricity share by tenant
+sms-0922-8866120</t>
+  </si>
+  <si>
+    <t>Bedrooms</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>Very Responsive</t>
+  </si>
+  <si>
+    <t>https://www.carousell.ph/p/smdc-shore-1-condosharing-condoshare-bedspace-1050627571/?t-id=7cWTSNfYfn_1613983964416&amp;t-referrer_browse_type=search_results&amp;t-referrer_request_id=cpgHOfjJVmso6zHL&amp;t-referrer_search_query=bedspace&amp;t-referrer_sort_by=popular</t>
+  </si>
+  <si>
+    <t>https://media.karousell.com/media/photos/products/2020/11/21/smdc_shore_1_condosharing_cond_1605975877_55a6117b_progressive.jpg, https://media.karousell.com/media/photos/products/2020/11/21/smdc_shore_1_condosharing_cond_1605975878_fa868f2b_progressive.jpg, https://media.karousell.com/media/photos/products/2020/11/21/smdc_shore_1_condosharing_cond_1605975878_fab5c49b_progressive.jpg, https://media.karousell.com/media/photos/products/2020/11/21/smdc_shore_1_condosharing_cond_1605975878_5d24d3b3_progressive.jpg, https://media.karousell.com/media/photos/products/2020/11/21/smdc_shore_1_condosharing_cond_1605975878_ca54325c_progressive.jpg</t>
+  </si>
+  <si>
+    <t>Bedspace Near SM City Sta. Mesa and LRT 2 Station in V. Mapa</t>
+  </si>
+  <si>
+    <t>The Silk Residences Tower 1 In Ramon Magsaysay Blvd., Santol 
+Street, Sta Mesa, Manila.
+Studio 23 SQM
+Monthly Rent is 4,000. with Security Deposit 4,000.
+Accept : Female Bedspacers Only
+Minimum 6 months rent
+Call or Text : 0956 830 62 51</t>
+  </si>
+  <si>
+    <t>Verified</t>
+  </si>
+  <si>
+    <t>https://www.carousell.ph/p/bedspace-near-sm-city-sta-mesa-and-lrt-2-station-in-v-mapa-1041605403/?t-id=7cWTSNfYfn_1613983964416&amp;t-referrer_browse_type=search_results&amp;t-referrer_request_id=cpgHOfjJVmso6zHL&amp;t-referrer_search_query=bedspace&amp;t-referrer_sort_by=popular</t>
+  </si>
+  <si>
+    <t>https://media.karousell.com/media/photos/products/2020/10/13/bedspace_near_sm_city_sta_mesa_1602584117_ffa0af5f_progressive, https://media.karousell.com/media/photos/products/2020/10/13/bedspace_near_sm_city_sta_mesa_1602584117_ea522cf9_progressive, https://media.karousell.com/media/photos/products/2020/10/13/bedspace_near_sm_city_sta_mesa_1602584117_21f755a3_progressive, https://media.karousell.com/media/photos/products/2020/10/13/bedspace_near_sm_city_sta_mesa_1602584117_0201b241_progressive, https://media.karousell.com/media/photos/products/2020/10/13/bedspace_near_sm_city_sta_mesa_1602584117_34eaece8_progressive, https://media.karousell.com/media/photos/products/2020/10/13/bedspace_near_sm_city_sta_mesa_1602584117_c12c8587_progressive, https://media.karousell.com/media/photos/products/2020/10/13/bedspace_near_sm_city_sta_mesa_1602584117_2ff165fc_progressive, https://media.karousell.com/media/photos/products/2020/10/13/bedspace_near_sm_city_sta_mesa_1602584117_829d6b4a_progressive, https://media.karousell.com/media/photos/products/2020/10/13/bedspace_near_sm_city_sta_mesa_1602584117_c21b81cd_progressive, https://media.karousell.com/media/photos/products/2020/10/13/bedspace_near_sm_city_sta_mesa_1602584117_03a1c006_progressive</t>
+  </si>
+  <si>
+    <t>SMDC Mezza residences condoshare bedspace Condosharing</t>
+  </si>
+  <si>
+    <t>SMDC Mezza residences -in front of CCP, near UERM, SM sta mezA, MRT sta, along aurora Blvd.
+Tower 3, 36th floor penthouse
+3 bedroom-3 toilet
+need 3 females in one room
+p4000 / bedspace/per head
+inclusive condo dues.
+water &amp; electricity share by tenant
+SMS -0922-8866120</t>
+  </si>
+  <si>
+    <t>https://www.carousell.ph/p/smdc-mezza-residences-condoshare-bedspace-condosharing-1050607145/?t-id=7cWTSNfYfn_1613983964416&amp;t-referrer_browse_type=search_results&amp;t-referrer_request_id=cpgHOfjJVmso6zHL&amp;t-referrer_search_query=bedspace&amp;t-referrer_sort_by=popular</t>
+  </si>
+  <si>
+    <t>https://media.karousell.com/media/photos/products/2020/11/21/smdc_mezza_residences_condosha_1605970200_5063a23a_progressive.jpg, https://media.karousell.com/media/photos/products/2020/11/21/smdc_mezza_residences_condosha_1605970201_f73f8320_progressive.jpg, https://media.karousell.com/media/photos/products/2020/11/21/smdc_mezza_residences_condosha_1605970201_df18f45f_progressive.jpg, https://media.karousell.com/media/photos/products/2020/11/21/smdc_mezza_residences_condosha_1605970201_423efd75_progressive.jpg, https://media.karousell.com/media/photos/products/2020/11/21/smdc_mezza_residences_condosha_1605970201_ccf5787b_progressive.jpg, https://media.karousell.com/media/photos/products/2020/11/21/smdc_mezza_residences_condosha_1605970201_dafc109f_progressive.jpg, https://media.karousell.com/media/photos/products/2020/11/21/smdc_mezza_residences_condosha_1605970202_c52ad49b_progressive.jpg</t>
+  </si>
+  <si>
+    <t>Bedspace for Rent - Ladies</t>
+  </si>
+  <si>
+    <t>Female Bedspace for Rent near San Andres Malate, Manila
+-Exclusive for Ladies
+-Php 2,500/month
+-Electricity and water already included in the rent
+-No curfew
+-Convenient location for people applying to work abroad, employees, OJT students
+Message us for more details.</t>
+  </si>
+  <si>
+    <t>https://www.carousell.ph/p/bedspace-for-rent-ladies-239185562/?t-id=7cWTSNfYfn_1613983964416&amp;t-referrer_browse_type=search_results&amp;t-referrer_request_id=cpgHOfjJVmso6zHL&amp;t-referrer_search_query=bedspace&amp;t-referrer_sort_by=popular</t>
+  </si>
+  <si>
+    <t>https://media.karousell.com/media/photos/products/2019/11/23/bedspace_for_rent__ladies_1574473718_d52b1828_progressive.jpg, https://media.karousell.com/media/photos/products/2019/11/23/bedspace_for_rent__ladies_1574473718_48af0582_progressive.jpg, https://media.karousell.com/media/photos/products/2019/11/23/bedspace_for_rent__ladies_1574473718_3aec2437_progressive.jpg, https://media.karousell.com/media/photos/products/2019/11/23/bedspace_for_rent__ladies_1574473718_b68230bc_progressive.jpg, https://media.karousell.com/media/photos/products/2019/11/23/bedspace_for_rent__ladies_1574473718_33535da3_progressive.jpg</t>
+  </si>
+  <si>
+    <t>Bedspace For Male Mandaluyong</t>
+  </si>
+  <si>
+    <t>Rm Solo/Shared 
+Initial Paymt: 4-Gives or P500 ONLY
+Monthly Rent: 2-Gives
+Looking For: Male Young Professionals (Decent)
+Age: 20-45
+Reqs.: (ID Pix, Co. ID, Any Gov't ID, NBI Clearance) 
+Various Perks and Privileges: 
+1. The whole townhouse unit is usable, with ac, fully furnished 
+2. No Curfew, gate/Rm keys provided 
+3. 24-hours water supply &amp; transportation
+4. Housekeeper's Provided
+5. Free Pick-up and Delivery of Laundry Services 
+6. Group WIFI access 
+7. Free Parking space 
+8. Accessible to all primary needs
+9. Events &amp; Activities 
+10.Various Discounts 
+For more details, u may text me at 0917-5113088. U may visit d place 2 appreciate &amp; we will discuss all the perks and privileges. - MARC</t>
+  </si>
+  <si>
+    <t>https://www.carousell.ph/p/bedspace-for-male-mandaluyong-238486060/?t-id=7cWTSNfYfn_1613983964416&amp;t-referrer_browse_type=search_results&amp;t-referrer_request_id=cpgHOfjJVmso6zHL&amp;t-referrer_search_query=bedspace&amp;t-referrer_sort_by=popular</t>
+  </si>
+  <si>
+    <t>https://media.karousell.com/media/photos/products/2019/07/11/230654_238486060_b00edfa7.jpg, https://media.karousell.com/media/photos/products/2019/07/11/230654_238486060_719e1e68.jpg, https://media.karousell.com/media/photos/products/2019/07/11/230654_238486060_32f21557.jpg, https://media.karousell.com/media/photos/products/2019/07/11/230654_238486060_d1d2e999.jpg, https://media.karousell.com/media/photos/products/2019/07/11/230654_238486060_1f516216.jpg, https://media.karousell.com/media/photos/products/2019/07/11/230654_238486060_e85abcd2.jpg, https://media.karousell.com/media/photos/products/2019/07/11/230654_238486060_94745904.jpg, https://media.karousell.com/media/photos/products/2019/07/11/230654_238486060_89f02bb9.jpg, https://media.karousell.com/media/photos/products/2019/07/11/230654_238486060_fa0dfc30.jpg, https://media.karousell.com/media/photos/products/2019/07/11/230654_238486060_9c7c6ccf.jpg</t>
+  </si>
+  <si>
+    <t>Moonwalk Paranaque Bedspace for rent</t>
+  </si>
+  <si>
+    <t>*Prices is per head
+*Free water and electric 
+(Shower and Fan only *NO LAUNDRY ALLOWED)
+*Near Mcdo Moonwalk
+*Near 7-11 &amp; other 24/hrs convenient store
+*Near BDO 
+*Near SM Sucat and Bicutan
+*ONLY 2 person in each room
+*We also accept short term/transient (please call/txt for inquiry)</t>
+  </si>
+  <si>
+    <t>https://www.carousell.ph/p/moonwalk-paranaque-bedspace-for-rent-243185456/?t-id=7cWTSNfYfn_1613983964416&amp;t-referrer_browse_type=search_results&amp;t-referrer_request_id=cpgHOfjJVmso6zHL&amp;t-referrer_search_query=bedspace&amp;t-referrer_sort_by=popular</t>
+  </si>
+  <si>
+    <t>https://media.karousell.com/media/photos/products/2019/08/01/153441_243185456_d560711a.jpg, https://media.karousell.com/media/photos/products/2019/08/01/153441_243185456_452021d1.jpg, https://media.karousell.com/media/photos/products/2019/08/01/153441_243185456_f52bbf05.jpg</t>
+  </si>
+  <si>
+    <t>Condo Sharing Bedspace</t>
+  </si>
+  <si>
+    <t>4,500php per month. All in kasama na tubig at kuryente, Aircon room, wifi and own CR wala ng ibang babayaran provided na din ung bed at ibang gamit, kahit damit nalang dalhin mo. 
+Sa second floor po ung room, 
+Downstairs naman ung kitchen, w/ refrigerator,microwave, rice cooker &amp; electric kettle.
+Free use of pool, gym and other facilities.
+Bedspace po ito. For FEMALE ONLY!!
+Location: Gateway Garden heights sa tabi lang Ng Robinson's forum kaya marami Ka mabibilhan Ng pagkaen. Malapit din sa lahat Ng sakayan kaya wala Ng masyadong lakad.
+Para sa mga interesado paki message nalang ako sa FB account ko... 
+Lanzce Descartin
+Thanks, God bless.</t>
+  </si>
+  <si>
+    <t>https://www.carousell.ph/p/condo-sharing-bedspace-243190069/?t-id=7cWTSNfYfn_1613983964416&amp;t-referrer_browse_type=search_results&amp;t-referrer_request_id=cpgHOfjJVmso6zHL&amp;t-referrer_search_query=bedspace&amp;t-referrer_sort_by=popular</t>
+  </si>
+  <si>
+    <t>https://media.karousell.com/media/photos/products/2019/08/01/155610_243190069_2e685974.jpg, https://media.karousell.com/media/photos/products/2019/08/01/155610_243190069_1f4881f0.jpg, https://media.karousell.com/media/photos/products/2019/08/01/155610_243190069_ad3dab89.jpg, https://media.karousell.com/media/photos/products/2019/08/01/155610_243190069_bff34032.jpg, https://media.karousell.com/media/photos/products/2019/08/01/155610_243190069_04030b0e.jpg, https://media.karousell.com/media/photos/products/2019/08/01/155610_243190069_b914c72a.jpg, https://media.karousell.com/media/photos/products/2019/08/01/155610_243190069_5bb01004.jpg, https://media.karousell.com/media/photos/products/2019/08/01/155610_243190069_f49243a7.jpg, https://media.karousell.com/media/photos/products/2019/08/01/155610_243190069_b750303f.jpg, https://media.karousell.com/media/photos/products/2019/08/01/155610_243190069_035f34e7.jpg</t>
   </si>
 </sst>
 </file>
@@ -160,6 +320,356 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5000.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="n">
+        <v>4000.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4500.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2500.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3000.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2700.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4500.0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P8" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>